<commit_message>
Actualización y Control Asignación
</commit_message>
<xml_diff>
--- a/Carga BF Voz (10).xlsx
+++ b/Carga BF Voz (10).xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/Nelson/Documents/REACT/evaluacion3/Proyecto-Evaluacion/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{5272495A-84FA-4F48-A937-667B4EB7D436}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{74E5B6B2-5A6B-BA4C-8D47-193DA96551D0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="6320" yWindow="1160" windowWidth="27240" windowHeight="16440" xr2:uid="{F167972B-225C-3A43-988D-0E5FF5725D1E}"/>
   </bookViews>
@@ -85,7 +85,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9020" uniqueCount="1030">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9053" uniqueCount="1033">
   <si>
     <t>Pais</t>
   </si>
@@ -3175,6 +3175,15 @@
   </si>
   <si>
     <t>00:11:18</t>
+  </si>
+  <si>
+    <t>Seguro1</t>
+  </si>
+  <si>
+    <t>Direccion1</t>
+  </si>
+  <si>
+    <t>Campo11</t>
   </si>
 </sst>
 </file>
@@ -4019,10 +4028,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BA461F6B-6533-5245-8118-B409AFC94560}">
-  <dimension ref="A1:Q81"/>
+  <dimension ref="A1:T81"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D8" sqref="D8"/>
+    <sheetView tabSelected="1" topLeftCell="D1" workbookViewId="0">
+      <selection activeCell="T9" sqref="T9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -4038,7 +4047,7 @@
     <col min="9" max="9" width="11.33203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:17" ht="30" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:20" ht="30" x14ac:dyDescent="0.2">
       <c r="A1" s="3" t="s">
         <v>969</v>
       </c>
@@ -4090,8 +4099,17 @@
       <c r="Q1" t="s">
         <v>1013</v>
       </c>
-    </row>
-    <row r="2" spans="1:17" s="13" customFormat="1" ht="15" x14ac:dyDescent="0.2">
+      <c r="R1" t="s">
+        <v>1030</v>
+      </c>
+      <c r="S1" t="s">
+        <v>1031</v>
+      </c>
+      <c r="T1" t="s">
+        <v>1032</v>
+      </c>
+    </row>
+    <row r="2" spans="1:20" s="13" customFormat="1" ht="15" x14ac:dyDescent="0.2">
       <c r="A2" s="13">
         <v>1</v>
       </c>
@@ -4143,8 +4161,17 @@
       <c r="Q2" s="13" t="s">
         <v>1014</v>
       </c>
-    </row>
-    <row r="3" spans="1:17" s="13" customFormat="1" ht="15" x14ac:dyDescent="0.2">
+      <c r="R2" s="13" t="s">
+        <v>1011</v>
+      </c>
+      <c r="S2" s="13" t="s">
+        <v>1012</v>
+      </c>
+      <c r="T2" s="13" t="s">
+        <v>1014</v>
+      </c>
+    </row>
+    <row r="3" spans="1:20" s="13" customFormat="1" ht="15" x14ac:dyDescent="0.2">
       <c r="A3" s="13">
         <v>2</v>
       </c>
@@ -4196,8 +4223,17 @@
       <c r="Q3" s="13" t="s">
         <v>1014</v>
       </c>
-    </row>
-    <row r="4" spans="1:17" s="13" customFormat="1" ht="15" x14ac:dyDescent="0.2">
+      <c r="R3" s="13" t="s">
+        <v>1011</v>
+      </c>
+      <c r="S3" s="13" t="s">
+        <v>1012</v>
+      </c>
+      <c r="T3" s="13" t="s">
+        <v>1014</v>
+      </c>
+    </row>
+    <row r="4" spans="1:20" s="13" customFormat="1" ht="15" x14ac:dyDescent="0.2">
       <c r="A4" s="13">
         <v>3</v>
       </c>
@@ -4249,8 +4285,17 @@
       <c r="Q4" s="13" t="s">
         <v>1014</v>
       </c>
-    </row>
-    <row r="5" spans="1:17" s="13" customFormat="1" ht="15" x14ac:dyDescent="0.2">
+      <c r="R4" s="13" t="s">
+        <v>1011</v>
+      </c>
+      <c r="S4" s="13" t="s">
+        <v>1012</v>
+      </c>
+      <c r="T4" s="13" t="s">
+        <v>1014</v>
+      </c>
+    </row>
+    <row r="5" spans="1:20" s="13" customFormat="1" ht="15" x14ac:dyDescent="0.2">
       <c r="A5" s="13">
         <v>4</v>
       </c>
@@ -4302,8 +4347,17 @@
       <c r="Q5" s="13" t="s">
         <v>1014</v>
       </c>
-    </row>
-    <row r="6" spans="1:17" s="13" customFormat="1" ht="15" x14ac:dyDescent="0.2">
+      <c r="R5" s="13" t="s">
+        <v>1011</v>
+      </c>
+      <c r="S5" s="13" t="s">
+        <v>1012</v>
+      </c>
+      <c r="T5" s="13" t="s">
+        <v>1014</v>
+      </c>
+    </row>
+    <row r="6" spans="1:20" s="13" customFormat="1" ht="15" x14ac:dyDescent="0.2">
       <c r="A6" s="13">
         <v>5</v>
       </c>
@@ -4355,8 +4409,17 @@
       <c r="Q6" s="13" t="s">
         <v>1014</v>
       </c>
-    </row>
-    <row r="7" spans="1:17" s="13" customFormat="1" ht="15" x14ac:dyDescent="0.2">
+      <c r="R6" s="13" t="s">
+        <v>1011</v>
+      </c>
+      <c r="S6" s="13" t="s">
+        <v>1012</v>
+      </c>
+      <c r="T6" s="13" t="s">
+        <v>1014</v>
+      </c>
+    </row>
+    <row r="7" spans="1:20" s="13" customFormat="1" ht="15" x14ac:dyDescent="0.2">
       <c r="A7" s="13">
         <v>6</v>
       </c>
@@ -4408,8 +4471,17 @@
       <c r="Q7" s="13" t="s">
         <v>1014</v>
       </c>
-    </row>
-    <row r="8" spans="1:17" s="13" customFormat="1" ht="15" x14ac:dyDescent="0.2">
+      <c r="R7" s="13" t="s">
+        <v>1011</v>
+      </c>
+      <c r="S7" s="13" t="s">
+        <v>1012</v>
+      </c>
+      <c r="T7" s="13" t="s">
+        <v>1014</v>
+      </c>
+    </row>
+    <row r="8" spans="1:20" s="13" customFormat="1" ht="15" x14ac:dyDescent="0.2">
       <c r="A8" s="13">
         <v>7</v>
       </c>
@@ -4461,8 +4533,17 @@
       <c r="Q8" s="13" t="s">
         <v>1014</v>
       </c>
-    </row>
-    <row r="9" spans="1:17" s="13" customFormat="1" ht="15" x14ac:dyDescent="0.2">
+      <c r="R8" s="13" t="s">
+        <v>1011</v>
+      </c>
+      <c r="S8" s="13" t="s">
+        <v>1012</v>
+      </c>
+      <c r="T8" s="13" t="s">
+        <v>1014</v>
+      </c>
+    </row>
+    <row r="9" spans="1:20" s="13" customFormat="1" ht="15" x14ac:dyDescent="0.2">
       <c r="A9" s="13">
         <v>8</v>
       </c>
@@ -4514,8 +4595,17 @@
       <c r="Q9" s="13" t="s">
         <v>1014</v>
       </c>
-    </row>
-    <row r="10" spans="1:17" s="13" customFormat="1" ht="15" x14ac:dyDescent="0.2">
+      <c r="R9" s="13" t="s">
+        <v>1011</v>
+      </c>
+      <c r="S9" s="13" t="s">
+        <v>1012</v>
+      </c>
+      <c r="T9" s="13" t="s">
+        <v>1014</v>
+      </c>
+    </row>
+    <row r="10" spans="1:20" s="13" customFormat="1" ht="15" x14ac:dyDescent="0.2">
       <c r="A10" s="13">
         <v>9</v>
       </c>
@@ -4567,8 +4657,17 @@
       <c r="Q10" s="13" t="s">
         <v>1014</v>
       </c>
-    </row>
-    <row r="11" spans="1:17" s="13" customFormat="1" ht="15" x14ac:dyDescent="0.2">
+      <c r="R10" s="13" t="s">
+        <v>1011</v>
+      </c>
+      <c r="S10" s="13" t="s">
+        <v>1012</v>
+      </c>
+      <c r="T10" s="13" t="s">
+        <v>1014</v>
+      </c>
+    </row>
+    <row r="11" spans="1:20" s="13" customFormat="1" ht="15" x14ac:dyDescent="0.2">
       <c r="A11" s="13">
         <v>10</v>
       </c>
@@ -4620,8 +4719,17 @@
       <c r="Q11" s="13" t="s">
         <v>1014</v>
       </c>
-    </row>
-    <row r="12" spans="1:17" s="13" customFormat="1" ht="15" x14ac:dyDescent="0.2">
+      <c r="R11" s="13" t="s">
+        <v>1011</v>
+      </c>
+      <c r="S11" s="13" t="s">
+        <v>1012</v>
+      </c>
+      <c r="T11" s="13" t="s">
+        <v>1014</v>
+      </c>
+    </row>
+    <row r="12" spans="1:20" s="13" customFormat="1" ht="15" x14ac:dyDescent="0.2">
       <c r="B12" s="1"/>
       <c r="C12" s="1"/>
       <c r="D12" s="33"/>
@@ -4632,7 +4740,7 @@
       <c r="I12" s="35"/>
       <c r="J12" s="10"/>
     </row>
-    <row r="13" spans="1:17" s="13" customFormat="1" ht="15" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:20" s="13" customFormat="1" ht="15" x14ac:dyDescent="0.2">
       <c r="B13" s="1"/>
       <c r="C13" s="1"/>
       <c r="D13" s="33"/>
@@ -4643,7 +4751,7 @@
       <c r="I13" s="35"/>
       <c r="J13" s="2"/>
     </row>
-    <row r="14" spans="1:17" s="13" customFormat="1" ht="15" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:20" s="13" customFormat="1" ht="15" x14ac:dyDescent="0.2">
       <c r="B14" s="1"/>
       <c r="C14" s="1"/>
       <c r="D14" s="33"/>
@@ -4654,7 +4762,7 @@
       <c r="I14" s="35"/>
       <c r="J14" s="2"/>
     </row>
-    <row r="15" spans="1:17" s="13" customFormat="1" ht="15" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:20" s="13" customFormat="1" ht="15" x14ac:dyDescent="0.2">
       <c r="B15" s="1"/>
       <c r="C15" s="1"/>
       <c r="D15" s="33"/>
@@ -4665,7 +4773,7 @@
       <c r="I15" s="35"/>
       <c r="J15" s="2"/>
     </row>
-    <row r="16" spans="1:17" s="13" customFormat="1" ht="15" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:20" s="13" customFormat="1" ht="15" x14ac:dyDescent="0.2">
       <c r="B16" s="1"/>
       <c r="C16" s="1"/>
       <c r="D16" s="33"/>

</xml_diff>